<commit_message>
Working kpis for displays
</commit_message>
<xml_diff>
--- a/Projects/PERNODUS/Data/Pernod_display_kpi.xlsx
+++ b/Projects/PERNODUS/Data/Pernod_display_kpi.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">brand_name</t>
   </si>
   <si>
-    <t xml:space="preserve">ABSOLUT,JAMESON,MALIBU,GLENLIVET,KAHULA,SEGRAMS,CHIVAS,AVION</t>
+    <t xml:space="preserve">ABSOLUT,JAMESON,MALIBU,GLENLIVET,KAHLUA,SEAGRAM'S,CHIVAS REGAL,AVION</t>
   </si>
   <si>
     <t xml:space="preserve">SHARE_OF_DISPLAY_MANUFACTURER</t>
@@ -223,7 +223,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -316,7 +316,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" s="1" customFormat="true" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -356,7 +356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -375,7 +375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Fixed kpis related to brand and template update
</commit_message>
<xml_diff>
--- a/Projects/PERNODUS/Data/Pernod_display_kpi.xlsx
+++ b/Projects/PERNODUS/Data/Pernod_display_kpi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t xml:space="preserve">KPI LEVEL 2</t>
   </si>
@@ -67,13 +67,7 @@
     <t xml:space="preserve">manufacturer_name</t>
   </si>
   <si>
-    <t xml:space="preserve">PERNOD RICARD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPIRITS</t>
+    <t xml:space="preserve">PERNOD RICARD,DIAGEO,BEAM SUNTORY,PROXIMO,BACARDI,E&amp;J GALLO,BROWN-FORMAN,CONSTELLATION,SAZERAC,HEAVEN HILL</t>
   </si>
   <si>
     <t xml:space="preserve">SOS_ON_DISPLAY_BRANDS</t>
@@ -82,7 +76,7 @@
     <t xml:space="preserve">brand_name</t>
   </si>
   <si>
-    <t xml:space="preserve">ABSOLUT,JAMESON,MALIBU,GLENLIVET,KAHLUA,SEAGRAM'S,CHIVAS REGAL,AVION</t>
+    <t xml:space="preserve">JAMESON,ABSOLUT,SEAGRAM'S,MALIBU,KAHLUA,GLENLIVET,CHIVAS REGAL,BEEFEATER,ALTOS,AVION,MARTELL,SMIRNOFF,TITO'S,NEW AMSTERDAM,CAPTAIN MORGAN,BACARDI,SAILOR JERRY,JACK DANIEL'S,JIM BEAM,MAKER'S MARK,JOSE CUERVO,SAUZA,1800,BAILEYS,JAGERMEISTER,CROWN ROYAL,FIREBALL,CANADIAN CLUB,BOMBAY,TANQUERAY,HENNESSY,COURVOISIER,REMY MARTIN,JOHNNIE WALKER</t>
   </si>
   <si>
     <t xml:space="preserve">SHARE_OF_DISPLAY_MANUFACTURER</t>
@@ -223,7 +217,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -308,23 +302,19 @@
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" s="1" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
@@ -335,7 +325,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -344,28 +334,24 @@
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="2"/>
       <c r="I6" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -375,16 +361,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>

</xml_diff>